<commit_message>
Started working on ChainLadder estimates.
</commit_message>
<xml_diff>
--- a/Design/EditorViewDesign.xlsx
+++ b/Design/EditorViewDesign.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="19020" windowHeight="9345" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="19020" windowHeight="9345" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Colors" sheetId="4" r:id="rId1"/>
     <sheet name="VectorEditor" sheetId="3" r:id="rId2"/>
     <sheet name="TriangleEditor" sheetId="2" r:id="rId3"/>
     <sheet name="ChainLadder" sheetId="1" r:id="rId4"/>
+    <sheet name="Bornhuetter-Ferguson" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
   <si>
     <t>Factors</t>
   </si>
@@ -152,13 +153,28 @@
   </si>
   <si>
     <t>developmentCount(int)</t>
+  </si>
+  <si>
+    <t>Loss ratios</t>
+  </si>
+  <si>
+    <t>Exposure</t>
+  </si>
+  <si>
+    <t>Accident</t>
+  </si>
+  <si>
+    <t>Reserve</t>
+  </si>
+  <si>
+    <t>Loss ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -194,6 +210,10 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1558,8 +1578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:N86"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView showGridLines="0" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52:G86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2251,4 +2271,747 @@
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:I94"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="3" spans="2:9">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="I3" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="I4" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="I5" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="I6" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="14"/>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="I29" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="B31" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="I36" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9">
+      <c r="B38" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="I38" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="B43" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="B44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" spans="2:9">
+      <c r="B45" s="9"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="11"/>
+    </row>
+    <row r="46" spans="2:9">
+      <c r="B46" s="9"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="11"/>
+    </row>
+    <row r="47" spans="2:9">
+      <c r="B47" s="9"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="11"/>
+    </row>
+    <row r="48" spans="2:9">
+      <c r="B48" s="9"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="11"/>
+    </row>
+    <row r="49" spans="2:7">
+      <c r="B49" s="9"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="11"/>
+    </row>
+    <row r="50" spans="2:7">
+      <c r="B50" s="12"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="14"/>
+    </row>
+    <row r="52" spans="2:7">
+      <c r="B52" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="2:7">
+      <c r="B53" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="8"/>
+    </row>
+    <row r="54" spans="2:7">
+      <c r="B54" s="9"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="11"/>
+    </row>
+    <row r="55" spans="2:7">
+      <c r="B55" s="9"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="11"/>
+    </row>
+    <row r="56" spans="2:7">
+      <c r="B56" s="9"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="11"/>
+    </row>
+    <row r="57" spans="2:7">
+      <c r="B57" s="9"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="11"/>
+    </row>
+    <row r="58" spans="2:7">
+      <c r="B58" s="12"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="14"/>
+    </row>
+    <row r="60" spans="2:7">
+      <c r="B60" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+    </row>
+    <row r="61" spans="2:7">
+      <c r="B61" s="6"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="8"/>
+    </row>
+    <row r="62" spans="2:7">
+      <c r="B62" s="9"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="11"/>
+    </row>
+    <row r="63" spans="2:7">
+      <c r="B63" s="9"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="11"/>
+    </row>
+    <row r="64" spans="2:7">
+      <c r="B64" s="9"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="11"/>
+    </row>
+    <row r="65" spans="2:7">
+      <c r="B65" s="9"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="11"/>
+    </row>
+    <row r="66" spans="2:7">
+      <c r="B66" s="9"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="11"/>
+    </row>
+    <row r="67" spans="2:7">
+      <c r="B67" s="12"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="14"/>
+    </row>
+    <row r="69" spans="2:7">
+      <c r="B69" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+    </row>
+    <row r="70" spans="2:7">
+      <c r="B70" s="6"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="8"/>
+    </row>
+    <row r="71" spans="2:7">
+      <c r="B71" s="9"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="11"/>
+    </row>
+    <row r="72" spans="2:7">
+      <c r="B72" s="9"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="11"/>
+    </row>
+    <row r="73" spans="2:7">
+      <c r="B73" s="9"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="11"/>
+    </row>
+    <row r="74" spans="2:7">
+      <c r="B74" s="9"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="11"/>
+    </row>
+    <row r="75" spans="2:7">
+      <c r="B75" s="9"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
+      <c r="G75" s="11"/>
+    </row>
+    <row r="76" spans="2:7">
+      <c r="B76" s="12"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="14"/>
+    </row>
+    <row r="78" spans="2:7">
+      <c r="B78" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+    </row>
+    <row r="79" spans="2:7">
+      <c r="B79" s="6"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="8"/>
+    </row>
+    <row r="80" spans="2:7">
+      <c r="B80" s="9"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="10"/>
+      <c r="G80" s="11"/>
+    </row>
+    <row r="81" spans="2:7">
+      <c r="B81" s="9"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="10"/>
+      <c r="G81" s="11"/>
+    </row>
+    <row r="82" spans="2:7">
+      <c r="B82" s="9"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="10"/>
+      <c r="G82" s="11"/>
+    </row>
+    <row r="83" spans="2:7">
+      <c r="B83" s="9"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10"/>
+      <c r="G83" s="11"/>
+    </row>
+    <row r="84" spans="2:7">
+      <c r="B84" s="9"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="10"/>
+      <c r="G84" s="11"/>
+    </row>
+    <row r="85" spans="2:7">
+      <c r="B85" s="12"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="14"/>
+    </row>
+    <row r="87" spans="2:7">
+      <c r="B87" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C87" s="15"/>
+      <c r="D87" s="15"/>
+      <c r="E87" s="15"/>
+      <c r="F87" s="15"/>
+      <c r="G87" s="15"/>
+    </row>
+    <row r="88" spans="2:7">
+      <c r="B88" s="6"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="7"/>
+      <c r="F88" s="7"/>
+      <c r="G88" s="8"/>
+    </row>
+    <row r="89" spans="2:7">
+      <c r="B89" s="9"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="11"/>
+    </row>
+    <row r="90" spans="2:7">
+      <c r="B90" s="9"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="11"/>
+    </row>
+    <row r="91" spans="2:7">
+      <c r="B91" s="9"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="10"/>
+      <c r="G91" s="11"/>
+    </row>
+    <row r="92" spans="2:7">
+      <c r="B92" s="9"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="10"/>
+      <c r="E92" s="10"/>
+      <c r="F92" s="10"/>
+      <c r="G92" s="11"/>
+    </row>
+    <row r="93" spans="2:7">
+      <c r="B93" s="9"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="10"/>
+      <c r="F93" s="10"/>
+      <c r="G93" s="11"/>
+    </row>
+    <row r="94" spans="2:7">
+      <c r="B94" s="12"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="13"/>
+      <c r="G94" s="14"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>